<commit_message>
actualizacion 7 de Marzo
</commit_message>
<xml_diff>
--- a/Resultado/informe_mensual_febrero.xlsx
+++ b/Resultado/informe_mensual_febrero.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slenis.BANCOLOMBIA\Documents\projecto_dashboard\Resultado\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E0BC95-63E2-448D-B601-59F1D654FE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Indicador</t>
   </si>
@@ -131,13 +150,28 @@
   </si>
   <si>
     <t>22.0%</t>
+  </si>
+  <si>
+    <t>Número de transacciones</t>
+  </si>
+  <si>
+    <t>Valor transacciones</t>
+  </si>
+  <si>
+    <t>6,607,677,129,791</t>
+  </si>
+  <si>
+    <t>7,421,985,990,886</t>
+  </si>
+  <si>
+    <t>14,029,663,120,677</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,13 +234,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -244,7 +286,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -278,6 +320,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -312,9 +355,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -487,14 +531,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:D21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,7 +554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -522,7 +568,7 @@
         <v>17170</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -536,7 +582,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -550,7 +596,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -564,7 +610,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -578,7 +624,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -592,7 +638,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -606,7 +652,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -620,7 +666,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -634,7 +680,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -648,7 +694,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -662,7 +708,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -676,7 +722,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -690,7 +736,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -704,7 +750,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -718,7 +764,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -732,7 +778,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -746,7 +792,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -758,6 +804,34 @@
       </c>
       <c r="D19">
         <v>1.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20">
+        <v>19411918</v>
+      </c>
+      <c r="C20">
+        <v>22301752</v>
+      </c>
+      <c r="D20">
+        <v>41713670</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>